<commit_message>
Inclusao da contagem na tabela dinamica
</commit_message>
<xml_diff>
--- a/_02_analises/Base_Inadimplencia_analises.xlsx
+++ b/_02_analises/Base_Inadimplencia_analises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinicius/Desktop/Mentorias/Github/exemplo/projeto_inadimplencia/_02_analises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B439313-86EC-8E45-837B-8F4D7816B149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4948C0-9894-C047-95DE-CC4D0E2E607C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{88496769-53D9-5B40-A32C-5DCB4B2AFDF9}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="18" r:id="rId4"/>
+    <pivotCache cacheId="20" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5035" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5036" uniqueCount="37">
   <si>
     <t>Variável</t>
   </si>
@@ -173,6 +173,9 @@
   <si>
     <t>Média de Inadimplencia</t>
   </si>
+  <si>
+    <t>Contagem de Escolaridade</t>
+  </si>
 </sst>
 </file>
 
@@ -251,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -266,11 +269,27 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -11353,12 +11372,12 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EC81EE6C-0B4B-8340-9F25-66B33D0E87AD}" name="Tabela dinâmica7" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EC81EE6C-0B4B-8340-9F25-66B33D0E87AD}" name="Tabela dinâmica7" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="4">
         <item x="2"/>
         <item x="0"/>
@@ -11396,14 +11415,23 @@
       <x/>
     </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
   </colItems>
-  <dataFields count="1">
+  <dataFields count="2">
     <dataField name="Média de Inadimplencia" fld="8" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
+    <dataField name="Contagem de Escolaridade" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="1">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -11412,7 +11440,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -40889,56 +40917,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DCEAF2-F312-124D-8C5C-3A4AD558B4BB}">
-  <dimension ref="A3:B7"/>
+  <dimension ref="A3:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="9">
         <v>0.3411764705882353</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="11">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="7">
         <v>0.29523809523809524</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="10">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="7">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="7">
         <v>0.3</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>